<commit_message>
Commit for missing values bug
</commit_message>
<xml_diff>
--- a/analysis_output/correlation_matrix.xlsx
+++ b/analysis_output/correlation_matrix.xlsx
@@ -500,34 +500,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.585</v>
+        <v>0.596</v>
       </c>
       <c r="D2" t="n">
-        <v>0.147</v>
+        <v>0.172</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.03</v>
+        <v>-0.016</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.118</v>
+        <v>-0.119</v>
       </c>
       <c r="G2" t="n">
-        <v>0.051</v>
+        <v>0.067</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.136</v>
+        <v>-0.111</v>
       </c>
       <c r="I2" t="n">
-        <v>0.135</v>
+        <v>0.152</v>
       </c>
       <c r="J2" t="n">
-        <v>0.117</v>
+        <v>0.14</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.123</v>
+        <v>-0.127</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.001</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="3">
@@ -537,37 +537,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.585</v>
+        <v>0.596</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.162</v>
+        <v>0.197</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.306</v>
+        <v>-0.276</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.386</v>
+        <v>-0.352</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.034</v>
+        <v>-0.012</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03</v>
+        <v>0.047</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.053</v>
+        <v>-0.018</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.063</v>
+        <v>-0.047</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.09</v>
+        <v>-0.092</v>
       </c>
       <c r="L3" t="n">
-        <v>0.127</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="4">
@@ -577,37 +577,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.147</v>
+        <v>0.172</v>
       </c>
       <c r="C4" t="n">
-        <v>0.162</v>
+        <v>0.197</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.467</v>
+        <v>0.479</v>
       </c>
       <c r="F4" t="n">
-        <v>0.039</v>
+        <v>0.073</v>
       </c>
       <c r="G4" t="n">
-        <v>0.618</v>
+        <v>0.622</v>
       </c>
       <c r="H4" t="n">
-        <v>0.319</v>
+        <v>0.318</v>
       </c>
       <c r="I4" t="n">
-        <v>0.407</v>
+        <v>0.423</v>
       </c>
       <c r="J4" t="n">
-        <v>0.358</v>
+        <v>0.357</v>
       </c>
       <c r="K4" t="n">
-        <v>0.08</v>
+        <v>0.095</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.052</v>
+        <v>-0.067</v>
       </c>
     </row>
     <row r="5">
@@ -617,37 +617,37 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.03</v>
+        <v>-0.016</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.306</v>
+        <v>-0.276</v>
       </c>
       <c r="D5" t="n">
-        <v>0.467</v>
+        <v>0.479</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.658</v>
+        <v>0.646</v>
       </c>
       <c r="G5" t="n">
-        <v>0.622</v>
+        <v>0.626</v>
       </c>
       <c r="H5" t="n">
-        <v>0.343</v>
+        <v>0.339</v>
       </c>
       <c r="I5" t="n">
-        <v>0.477</v>
+        <v>0.484</v>
       </c>
       <c r="J5" t="n">
-        <v>0.422</v>
+        <v>0.423</v>
       </c>
       <c r="K5" t="n">
-        <v>0.145</v>
+        <v>0.158</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.151</v>
+        <v>-0.162</v>
       </c>
     </row>
     <row r="6">
@@ -657,37 +657,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.118</v>
+        <v>-0.119</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.386</v>
+        <v>-0.352</v>
       </c>
       <c r="D6" t="n">
-        <v>0.039</v>
+        <v>0.073</v>
       </c>
       <c r="E6" t="n">
-        <v>0.658</v>
+        <v>0.646</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.25</v>
+        <v>0.257</v>
       </c>
       <c r="H6" t="n">
-        <v>0.219</v>
+        <v>0.218</v>
       </c>
       <c r="I6" t="n">
-        <v>0.302</v>
+        <v>0.297</v>
       </c>
       <c r="J6" t="n">
-        <v>0.231</v>
+        <v>0.209</v>
       </c>
       <c r="K6" t="n">
-        <v>0.199</v>
+        <v>0.213</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.281</v>
+        <v>-0.287</v>
       </c>
     </row>
     <row r="7">
@@ -697,37 +697,37 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.051</v>
+        <v>0.067</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.034</v>
+        <v>-0.012</v>
       </c>
       <c r="D7" t="n">
-        <v>0.618</v>
+        <v>0.622</v>
       </c>
       <c r="E7" t="n">
-        <v>0.622</v>
+        <v>0.626</v>
       </c>
       <c r="F7" t="n">
-        <v>0.25</v>
+        <v>0.257</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.375</v>
+        <v>0.381</v>
       </c>
       <c r="I7" t="n">
-        <v>0.35</v>
+        <v>0.354</v>
       </c>
       <c r="J7" t="n">
-        <v>0.305</v>
+        <v>0.312</v>
       </c>
       <c r="K7" t="n">
-        <v>0.004</v>
+        <v>0.016</v>
       </c>
       <c r="L7" t="n">
-        <v>0.036</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="8">
@@ -737,37 +737,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.136</v>
+        <v>-0.111</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03</v>
+        <v>0.047</v>
       </c>
       <c r="D8" t="n">
-        <v>0.319</v>
+        <v>0.318</v>
       </c>
       <c r="E8" t="n">
-        <v>0.343</v>
+        <v>0.339</v>
       </c>
       <c r="F8" t="n">
-        <v>0.219</v>
+        <v>0.218</v>
       </c>
       <c r="G8" t="n">
-        <v>0.375</v>
+        <v>0.381</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04</v>
+        <v>0.037</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1</v>
+        <v>0.115</v>
       </c>
       <c r="K8" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.032</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="9">
@@ -777,37 +777,37 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.135</v>
+        <v>0.152</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.053</v>
+        <v>-0.018</v>
       </c>
       <c r="D9" t="n">
-        <v>0.407</v>
+        <v>0.423</v>
       </c>
       <c r="E9" t="n">
-        <v>0.477</v>
+        <v>0.484</v>
       </c>
       <c r="F9" t="n">
-        <v>0.302</v>
+        <v>0.297</v>
       </c>
       <c r="G9" t="n">
-        <v>0.35</v>
+        <v>0.354</v>
       </c>
       <c r="H9" t="n">
-        <v>0.04</v>
+        <v>0.037</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.616</v>
+        <v>0.601</v>
       </c>
       <c r="K9" t="n">
         <v>0.021</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.318</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="10">
@@ -817,37 +817,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.117</v>
+        <v>0.14</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.063</v>
+        <v>-0.047</v>
       </c>
       <c r="D10" t="n">
-        <v>0.358</v>
+        <v>0.357</v>
       </c>
       <c r="E10" t="n">
-        <v>0.422</v>
+        <v>0.423</v>
       </c>
       <c r="F10" t="n">
-        <v>0.231</v>
+        <v>0.209</v>
       </c>
       <c r="G10" t="n">
-        <v>0.305</v>
+        <v>0.312</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1</v>
+        <v>0.115</v>
       </c>
       <c r="I10" t="n">
-        <v>0.616</v>
+        <v>0.601</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.109</v>
+        <v>-0.099</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.231</v>
+        <v>-0.222</v>
       </c>
     </row>
     <row r="11">
@@ -857,37 +857,37 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.123</v>
+        <v>-0.127</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.09</v>
+        <v>-0.092</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08</v>
+        <v>0.095</v>
       </c>
       <c r="E11" t="n">
-        <v>0.145</v>
+        <v>0.158</v>
       </c>
       <c r="F11" t="n">
-        <v>0.199</v>
+        <v>0.213</v>
       </c>
       <c r="G11" t="n">
-        <v>0.004</v>
+        <v>0.016</v>
       </c>
       <c r="H11" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
       <c r="I11" t="n">
         <v>0.021</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.109</v>
+        <v>-0.099</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.022</v>
+        <v>-0.047</v>
       </c>
     </row>
     <row r="12">
@@ -897,34 +897,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.001</v>
+        <v>0.014</v>
       </c>
       <c r="C12" t="n">
-        <v>0.127</v>
+        <v>0.137</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.052</v>
+        <v>-0.067</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.151</v>
+        <v>-0.162</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.281</v>
+        <v>-0.287</v>
       </c>
       <c r="G12" t="n">
-        <v>0.036</v>
+        <v>0.029</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.032</v>
+        <v>-0.02</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.318</v>
+        <v>-0.31</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.231</v>
+        <v>-0.222</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.022</v>
+        <v>-0.047</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>

</xml_diff>